<commit_message>
atualizando tabela e adicionando status do time no campeonato
</commit_message>
<xml_diff>
--- a/data/brasileirao2023.xlsx
+++ b/data/brasileirao2023.xlsx
@@ -4003,9 +4003,15 @@
       <c r="C182" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D182" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E182" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F182" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2">
@@ -4017,9 +4023,15 @@
       <c r="C183" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D183" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E183" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F183" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2">
@@ -4031,9 +4043,15 @@
       <c r="C184" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D184" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E184" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F184" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="2">
@@ -4045,9 +4063,15 @@
       <c r="C185" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D185" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E185" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F185" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2">
@@ -4059,9 +4083,15 @@
       <c r="C186" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D186" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E186" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F186" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="2">
@@ -4073,9 +4103,15 @@
       <c r="C187" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D187" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E187" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F187" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="2">
@@ -4087,9 +4123,15 @@
       <c r="C188" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D188" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E188" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F188" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2">
@@ -4101,9 +4143,15 @@
       <c r="C189" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D189" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E189" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F189" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2">
@@ -4115,9 +4163,15 @@
       <c r="C190" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D190" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E190" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F190" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2">
@@ -4129,9 +4183,15 @@
       <c r="C191" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D191" s="2">
+        <v>4.0</v>
+      </c>
       <c r="E191" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F191" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2">
@@ -4143,9 +4203,15 @@
       <c r="C192" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D192" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E192" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F192" s="2">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2">
@@ -4157,9 +4223,15 @@
       <c r="C193" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D193" s="2">
+        <v>4.0</v>
+      </c>
       <c r="E193" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F193" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="2">
@@ -4171,9 +4243,15 @@
       <c r="C194" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D194" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E194" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F194" s="2">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="2">
@@ -4185,9 +4263,15 @@
       <c r="C195" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D195" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E195" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F195" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="2">
@@ -4199,9 +4283,15 @@
       <c r="C196" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D196" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E196" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F196" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="2">
@@ -4213,9 +4303,15 @@
       <c r="C197" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D197" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E197" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F197" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="2">
@@ -4227,9 +4323,15 @@
       <c r="C198" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D198" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E198" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="F198" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="2">
@@ -4241,9 +4343,15 @@
       <c r="C199" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D199" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E199" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F199" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="2">
@@ -4255,9 +4363,15 @@
       <c r="C200" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D200" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E200" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F200" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="2">
@@ -4269,8 +4383,14 @@
       <c r="C201" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D201" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E201" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F201" s="2">
+        <v>1.0</v>
       </c>
     </row>
     <row r="202">

</xml_diff>

<commit_message>
feat: adicionado arquivos teste
</commit_message>
<xml_diff>
--- a/data/brasileirao2023.xlsx
+++ b/data/brasileirao2023.xlsx
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -157,6 +157,7 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3263,15 +3264,11 @@
       <c r="C145" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D145" s="5">
-        <v>0.0</v>
-      </c>
+      <c r="D145" s="5"/>
       <c r="E145" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F145" s="5">
-        <v>0.0</v>
-      </c>
+      <c r="F145" s="5"/>
     </row>
     <row r="146">
       <c r="A146" s="2">
@@ -3383,15 +3380,11 @@
       <c r="C151" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D151" s="5">
-        <v>0.0</v>
-      </c>
+      <c r="D151" s="5"/>
       <c r="E151" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F151" s="5">
-        <v>0.0</v>
-      </c>
+      <c r="F151" s="5"/>
     </row>
     <row r="152">
       <c r="A152" s="2">
@@ -4403,9 +4396,15 @@
       <c r="C202" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D202" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E202" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F202" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="2">
@@ -4417,9 +4416,15 @@
       <c r="C203" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D203" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E203" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F203" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="2">
@@ -4431,9 +4436,15 @@
       <c r="C204" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D204" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E204" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F204" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="2">
@@ -4445,9 +4456,15 @@
       <c r="C205" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D205" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E205" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F205" s="2">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="2">
@@ -4459,9 +4476,15 @@
       <c r="C206" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D206" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E206" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F206" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="2">
@@ -4473,9 +4496,15 @@
       <c r="C207" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D207" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E207" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F207" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="2">
@@ -4487,9 +4516,15 @@
       <c r="C208" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D208" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E208" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F208" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="2">
@@ -4501,9 +4536,15 @@
       <c r="C209" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D209" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E209" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F209" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2">
@@ -4515,9 +4556,15 @@
       <c r="C210" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D210" s="2">
+        <v>3.0</v>
+      </c>
       <c r="E210" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F210" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2">
@@ -4529,9 +4576,15 @@
       <c r="C211" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D211" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E211" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F211" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="2">
@@ -4543,9 +4596,11 @@
       <c r="C212" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D212" s="6"/>
       <c r="E212" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F212" s="6"/>
     </row>
     <row r="213">
       <c r="A213" s="2">
@@ -4557,9 +4612,15 @@
       <c r="C213" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D213" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E213" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F213" s="2">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2">
@@ -4571,9 +4632,15 @@
       <c r="C214" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D214" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E214" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F214" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="2">
@@ -4585,9 +4652,15 @@
       <c r="C215" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D215" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E215" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F215" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="2">
@@ -4599,9 +4672,15 @@
       <c r="C216" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D216" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E216" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F216" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="2">
@@ -4613,9 +4692,15 @@
       <c r="C217" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D217" s="2">
+        <v>0.0</v>
+      </c>
       <c r="E217" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F217" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="2">
@@ -4627,9 +4712,15 @@
       <c r="C218" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D218" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E218" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="F218" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="2">
@@ -4641,9 +4732,15 @@
       <c r="C219" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D219" s="2">
+        <v>2.0</v>
+      </c>
       <c r="E219" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F219" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="2">
@@ -4655,9 +4752,15 @@
       <c r="C220" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D220" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E220" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F220" s="2">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="2">
@@ -4669,8 +4772,14 @@
       <c r="C221" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D221" s="2">
+        <v>1.0</v>
+      </c>
       <c r="E221" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F221" s="2">
+        <v>1.0</v>
       </c>
     </row>
     <row r="222">

</xml_diff>

<commit_message>
refactor: alterando cores e tamanhos
cores de tabela, título
</commit_message>
<xml_diff>
--- a/data/brasileirao2023.xlsx
+++ b/data/brasileirao2023.xlsx
@@ -109,7 +109,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -170,14 +170,14 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -504,7 +504,7 @@
     <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>2023</v>
       </c>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2023</v>
       </c>
@@ -564,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>2023</v>
       </c>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>2023</v>
       </c>
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
@@ -664,7 +664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>2023</v>
       </c>
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>2023</v>
       </c>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>2023</v>
       </c>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>2023</v>
       </c>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>2023</v>
       </c>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
         <v>2023</v>
       </c>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>2023</v>
       </c>
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
         <v>2023</v>
       </c>
@@ -824,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>2023</v>
       </c>
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3">
         <v>2023</v>
       </c>
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3">
         <v>2023</v>
       </c>
@@ -884,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3">
         <v>2023</v>
       </c>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3">
         <v>2023</v>
       </c>
@@ -924,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3">
         <v>2023</v>
       </c>
@@ -944,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3">
         <v>2023</v>
       </c>
@@ -964,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3">
         <v>2023</v>
       </c>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3">
         <v>2023</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3">
         <v>2023</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3">
         <v>2023</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3">
         <v>2023</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3">
         <v>2023</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3">
         <v>2023</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3">
         <v>2023</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3">
         <v>2023</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3">
         <v>2023</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="3">
         <v>2023</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3">
         <v>2023</v>
       </c>
@@ -5734,11 +5734,15 @@
       <c r="C262" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D262" s="5"/>
+      <c r="D262" s="5">
+        <v>1</v>
+      </c>
       <c r="E262" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F262" s="5"/>
+      <c r="F262" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="18.75">
       <c r="A263" s="3">
@@ -5750,11 +5754,15 @@
       <c r="C263" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D263" s="5"/>
+      <c r="D263" s="5">
+        <v>3</v>
+      </c>
       <c r="E263" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F263" s="5"/>
+      <c r="F263" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="18.75">
       <c r="A264" s="3">
@@ -5766,11 +5774,15 @@
       <c r="C264" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D264" s="5"/>
+      <c r="D264" s="5">
+        <v>0</v>
+      </c>
       <c r="E264" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F264" s="5"/>
+      <c r="F264" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="18.75">
       <c r="A265" s="3">
@@ -5782,11 +5794,15 @@
       <c r="C265" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D265" s="5"/>
+      <c r="D265" s="5">
+        <v>1</v>
+      </c>
       <c r="E265" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F265" s="5"/>
+      <c r="F265" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="18.75">
       <c r="A266" s="3">
@@ -5798,11 +5814,15 @@
       <c r="C266" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D266" s="5"/>
+      <c r="D266" s="5">
+        <v>1</v>
+      </c>
       <c r="E266" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F266" s="5"/>
+      <c r="F266" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="18.75">
       <c r="A267" s="3">
@@ -5814,11 +5834,15 @@
       <c r="C267" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D267" s="5"/>
+      <c r="D267" s="5">
+        <v>1</v>
+      </c>
       <c r="E267" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F267" s="5"/>
+      <c r="F267" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="18.75">
       <c r="A268" s="3">
@@ -5830,11 +5854,15 @@
       <c r="C268" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D268" s="5"/>
+      <c r="D268" s="5">
+        <v>0</v>
+      </c>
       <c r="E268" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F268" s="5"/>
+      <c r="F268" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="18.75">
       <c r="A269" s="3">
@@ -5846,11 +5874,15 @@
       <c r="C269" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D269" s="5"/>
+      <c r="D269" s="5">
+        <v>1</v>
+      </c>
       <c r="E269" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F269" s="5"/>
+      <c r="F269" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="270" customHeight="1" ht="18.75">
       <c r="A270" s="3">
@@ -5862,11 +5894,15 @@
       <c r="C270" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D270" s="5"/>
+      <c r="D270" s="5">
+        <v>0</v>
+      </c>
       <c r="E270" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F270" s="5"/>
+      <c r="F270" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="18.75">
       <c r="A271" s="3">
@@ -5878,11 +5914,15 @@
       <c r="C271" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D271" s="5"/>
+      <c r="D271" s="5">
+        <v>2</v>
+      </c>
       <c r="E271" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F271" s="5"/>
+      <c r="F271" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="272" customHeight="1" ht="18.75">
       <c r="A272" s="3">
@@ -5894,11 +5934,15 @@
       <c r="C272" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D272" s="5"/>
+      <c r="D272" s="5">
+        <v>1</v>
+      </c>
       <c r="E272" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F272" s="5"/>
+      <c r="F272" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="18.75">
       <c r="A273" s="3">
@@ -5910,11 +5954,15 @@
       <c r="C273" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D273" s="5"/>
+      <c r="D273" s="5">
+        <v>1</v>
+      </c>
       <c r="E273" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F273" s="5"/>
+      <c r="F273" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="274" customHeight="1" ht="18.75">
       <c r="A274" s="3">
@@ -5926,11 +5974,15 @@
       <c r="C274" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D274" s="5"/>
+      <c r="D274" s="5">
+        <v>2</v>
+      </c>
       <c r="E274" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F274" s="5"/>
+      <c r="F274" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="18.75">
       <c r="A275" s="3">
@@ -5942,11 +5994,15 @@
       <c r="C275" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D275" s="5"/>
+      <c r="D275" s="5">
+        <v>0</v>
+      </c>
       <c r="E275" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F275" s="5"/>
+      <c r="F275" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="18.75">
       <c r="A276" s="3">
@@ -5958,11 +6014,15 @@
       <c r="C276" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D276" s="5"/>
+      <c r="D276" s="5">
+        <v>7</v>
+      </c>
       <c r="E276" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F276" s="5"/>
+      <c r="F276" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="18.75">
       <c r="A277" s="3">
@@ -5974,11 +6034,15 @@
       <c r="C277" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D277" s="5"/>
+      <c r="D277" s="5">
+        <v>0</v>
+      </c>
       <c r="E277" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F277" s="5"/>
+      <c r="F277" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="278" customHeight="1" ht="18.75">
       <c r="A278" s="3">
@@ -5990,11 +6054,15 @@
       <c r="C278" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D278" s="5"/>
+      <c r="D278" s="5">
+        <v>1</v>
+      </c>
       <c r="E278" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F278" s="5"/>
+      <c r="F278" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="18.75">
       <c r="A279" s="3">
@@ -6006,11 +6074,15 @@
       <c r="C279" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D279" s="5"/>
+      <c r="D279" s="5">
+        <v>3</v>
+      </c>
       <c r="E279" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F279" s="5"/>
+      <c r="F279" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="280" customHeight="1" ht="18.75">
       <c r="A280" s="3">
@@ -6022,11 +6094,15 @@
       <c r="C280" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D280" s="5"/>
+      <c r="D280" s="5">
+        <v>1</v>
+      </c>
       <c r="E280" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F280" s="5"/>
+      <c r="F280" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="281" customHeight="1" ht="18.75">
       <c r="A281" s="3">
@@ -6038,11 +6114,15 @@
       <c r="C281" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D281" s="5"/>
+      <c r="D281" s="5">
+        <v>1</v>
+      </c>
       <c r="E281" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F281" s="5"/>
+      <c r="F281" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="18.75">
       <c r="A282" s="3">

</xml_diff>